<commit_message>
Full implementation of moltenprot and our 384-well plate now complete. Working on NAPRC next.
</commit_message>
<xml_diff>
--- a/platemap.xlsx
+++ b/platemap.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E484452-3FDE-4D3F-938C-A1D125FD74DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4040E6D1-43A7-4309-9C7F-9DEA9E5A3A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-1730" windowWidth="25820" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="34">
   <si>
     <t>empty</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>control</t>
-  </si>
-  <si>
-    <t>DIA200264</t>
   </si>
 </sst>
 </file>
@@ -510,17 +507,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="25" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1</v>
       </c>
@@ -594,7 +588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -671,7 +665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -748,7 +742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -825,7 +819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -902,7 +896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -979,7 +973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1056,7 +1050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1133,7 +1127,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1210,7 +1204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1287,7 +1281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1364,7 +1358,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1441,7 +1435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1518,7 +1512,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1595,7 +1589,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1672,7 +1666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1749,7 +1743,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1836,17 +1830,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="25" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1</v>
       </c>
@@ -1920,7 +1911,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1997,7 +1988,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2074,7 +2065,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2151,7 +2142,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2228,7 +2219,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2305,7 +2296,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2382,7 +2373,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2459,7 +2450,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2536,7 +2527,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2613,7 +2604,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2690,7 +2681,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2767,7 +2758,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2844,7 +2835,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2921,7 +2912,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2998,7 +2989,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3075,7 +3066,7 @@
         <v>8.4675439042151409E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>

</xml_diff>